<commit_message>
added webdriver manager jars
updated some code
</commit_message>
<xml_diff>
--- a/KeywordExcel/Keywords.xlsx
+++ b/KeywordExcel/Keywords.xlsx
@@ -48,9 +48,6 @@
     <t>close browser</t>
   </si>
   <si>
-    <t>verify signup link</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>verify forgot password link</t>
   </si>
 </sst>
 </file>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -482,13 +482,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -496,13 +496,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -510,13 +510,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -524,13 +524,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -538,13 +538,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -552,13 +552,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -566,13 +566,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -580,27 +580,27 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -608,13 +608,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>